<commit_message>
fix read file citad
</commit_message>
<xml_diff>
--- a/src/main/resources/bank-code-list.xlsx
+++ b/src/main/resources/bank-code-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5964E50-81EE-4D42-A65F-988B8FE1CA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A54288E-4F10-4E2A-86B5-7920370E002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7636" uniqueCount="2236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7568" uniqueCount="2233">
   <si>
     <r>
       <rPr>
@@ -22385,36 +22385,6 @@
         <family val="1"/>
       </rPr>
       <t>Năm Căn</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Ngân hàng Hợp tác xã Việt Nam (Co-Operative Bank Of Viet Nam)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>PGD Quảng Bình</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Gia lai</t>
     </r>
   </si>
 </sst>
@@ -22806,10 +22776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3820"/>
+  <dimension ref="A1:C3786"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A3779" workbookViewId="0">
+      <selection activeCell="G3789" sqref="G3789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -64466,380 +64436,6 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="3787" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3787" s="4">
-        <v>1901001</v>
-      </c>
-      <c r="B3787" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3787" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="3788" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3788" s="4">
-        <v>1901002</v>
-      </c>
-      <c r="B3788" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3788" s="3" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="3789" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3789" s="4">
-        <v>1901003</v>
-      </c>
-      <c r="B3789" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3789" s="3" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="3790" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3790" s="4">
-        <v>1901004</v>
-      </c>
-      <c r="B3790" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3790" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3791" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3791" s="2">
-        <v>15901001</v>
-      </c>
-      <c r="B3791" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3791" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3792" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3792" s="2">
-        <v>24901001</v>
-      </c>
-      <c r="B3792" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3792" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3793" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3793" s="2">
-        <v>25901001</v>
-      </c>
-      <c r="B3793" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3793" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3794" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3794" s="2">
-        <v>26901001</v>
-      </c>
-      <c r="B3794" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3794" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3795" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3795" s="2">
-        <v>27901001</v>
-      </c>
-      <c r="B3795" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3795" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3796" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3796" s="2">
-        <v>30901001</v>
-      </c>
-      <c r="B3796" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3796" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3797" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3797" s="2">
-        <v>31901001</v>
-      </c>
-      <c r="B3797" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3797" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3798" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3798" s="2">
-        <v>33901001</v>
-      </c>
-      <c r="B3798" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3798" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3799" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3799" s="2">
-        <v>34901001</v>
-      </c>
-      <c r="B3799" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3799" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3800" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3800" s="2">
-        <v>35901001</v>
-      </c>
-      <c r="B3800" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3800" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3801" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3801" s="2">
-        <v>36901001</v>
-      </c>
-      <c r="B3801" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3801" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3802" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3802" s="2">
-        <v>37901001</v>
-      </c>
-      <c r="B3802" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3802" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3803" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3803" s="2">
-        <v>38901001</v>
-      </c>
-      <c r="B3803" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3803" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3804" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3804" s="2">
-        <v>40901001</v>
-      </c>
-      <c r="B3804" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3804" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3805" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3805" s="2">
-        <v>42901001</v>
-      </c>
-      <c r="B3805" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3805" s="3" t="s">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="3806" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3806" s="2">
-        <v>44901001</v>
-      </c>
-      <c r="B3806" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3806" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3807" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3807" s="2">
-        <v>45901001</v>
-      </c>
-      <c r="B3807" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3807" s="3" t="s">
-        <v>2234</v>
-      </c>
-    </row>
-    <row r="3808" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3808" s="2">
-        <v>52901001</v>
-      </c>
-      <c r="B3808" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3808" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3809" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3809" s="2">
-        <v>60901001</v>
-      </c>
-      <c r="B3809" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3809" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3810" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3810" s="2">
-        <v>64901001</v>
-      </c>
-      <c r="B3810" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3810" s="3" t="s">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="3811" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3811" s="2">
-        <v>66901001</v>
-      </c>
-      <c r="B3811" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3811" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3812" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3812" s="2">
-        <v>68901001</v>
-      </c>
-      <c r="B3812" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3812" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3813" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3813" s="2">
-        <v>72901001</v>
-      </c>
-      <c r="B3813" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3813" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3814" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3814" s="2">
-        <v>75901001</v>
-      </c>
-      <c r="B3814" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3814" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3815" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3815" s="2">
-        <v>79901001</v>
-      </c>
-      <c r="B3815" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3815" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3816" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3816" s="2">
-        <v>80901001</v>
-      </c>
-      <c r="B3816" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3816" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3817" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3817" s="2">
-        <v>84901001</v>
-      </c>
-      <c r="B3817" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3817" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3818" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3818" s="2">
-        <v>89901001</v>
-      </c>
-      <c r="B3818" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3818" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3819" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3819" s="2">
-        <v>91901001</v>
-      </c>
-      <c r="B3819" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3819" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3820" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3820" s="2">
-        <v>94901001</v>
-      </c>
-      <c r="B3820" s="3" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C3820" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>